<commit_message>
Tatamotors announced a demerger so, made some changes in the input file.
</commit_message>
<xml_diff>
--- a/sample_portfolio.xlsx
+++ b/sample_portfolio.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krishvenigalla/Desktop/Private Equity/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D5AF18-B4FB-7141-BC20-E3DF7F49AC6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C021DD-AD1C-304E-B799-2CF4EB753001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="760" windowWidth="24960" windowHeight="16980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="1460" windowWidth="24960" windowHeight="16980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>Stock_Symbol</t>
   </si>
@@ -53,12 +53,6 @@
     <t>Total_Investment</t>
   </si>
   <si>
-    <t>TATAMOTORS</t>
-  </si>
-  <si>
-    <t>Tata Motors</t>
-  </si>
-  <si>
     <t>2024-01-15</t>
   </si>
   <si>
@@ -165,12 +159,27 @@
   </si>
   <si>
     <t>2024-05-01</t>
+  </si>
+  <si>
+    <t>TMCV</t>
+  </si>
+  <si>
+    <t>Tata Motors Limited</t>
+  </si>
+  <si>
+    <t>TMPV</t>
+  </si>
+  <si>
+    <t>Tata Motors Pass Vehicle Limited</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -183,6 +192,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -220,11 +230,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -527,13 +538,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -557,294 +571,313 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
       <c r="D2">
-        <v>398.42</v>
+        <v>124.11</v>
       </c>
       <c r="E2">
         <v>12</v>
       </c>
       <c r="F2">
-        <f>D2*E2</f>
-        <v>4781.04</v>
+        <v>1489.31</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
+        <v>45</v>
+      </c>
+      <c r="C3" s="2">
+        <v>45306</v>
       </c>
       <c r="D3">
-        <v>162.29</v>
+        <v>274.32</v>
       </c>
       <c r="E3">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F15" si="0">D3*E3</f>
-        <v>9412.82</v>
+        <v>3291.78</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D4">
-        <v>1489.48</v>
+        <v>162.29</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
-        <v>1489.48</v>
+        <f t="shared" ref="F4:F16" si="0">D4*E4</f>
+        <v>9412.82</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D5">
-        <v>889</v>
+        <v>1489.48</v>
       </c>
       <c r="E5">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>42672</v>
+        <v>1489.48</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D6">
-        <v>245.55</v>
+        <v>889</v>
       </c>
       <c r="E6">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>3683.25</v>
+        <v>42672</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D7">
-        <v>387.21</v>
+        <v>245.55</v>
       </c>
       <c r="E7">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>12777.929999999998</v>
+        <v>3683.25</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D8">
-        <v>261.31</v>
+        <v>387.21</v>
       </c>
       <c r="E8">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>10452.4</v>
+        <v>12777.929999999998</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D9">
-        <v>36.46</v>
+        <v>261.31</v>
       </c>
       <c r="E9">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>947.96</v>
+        <v>10452.4</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D10">
-        <v>152.47999999999999</v>
+        <v>36.46</v>
       </c>
       <c r="E10">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>762.4</v>
+        <v>947.96</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D11">
-        <v>910.09</v>
+        <v>152.47999999999999</v>
       </c>
       <c r="E11">
         <v>5</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>4550.45</v>
+        <v>762.4</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D12">
-        <v>324.48</v>
+        <v>910.09</v>
       </c>
       <c r="E12">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>4867.2000000000007</v>
+        <v>4550.45</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D13">
-        <v>743.38</v>
+        <v>324.48</v>
       </c>
       <c r="E13">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
-        <v>3716.9</v>
+        <v>4867.2000000000007</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D14">
-        <v>164.41</v>
+        <v>743.38</v>
       </c>
       <c r="E14">
-        <v>80</v>
+        <v>5</v>
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
-        <v>13152.8</v>
+        <v>3716.9</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15">
+        <v>164.41</v>
+      </c>
+      <c r="E15">
+        <v>80</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>13152.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
         <v>41</v>
       </c>
-      <c r="B15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15">
+      <c r="D16">
         <v>1032.26</v>
       </c>
-      <c r="E15">
+      <c r="E16">
         <v>3</v>
       </c>
-      <c r="F15">
+      <c r="F16">
         <f t="shared" si="0"/>
         <v>3096.7799999999997</v>
       </c>

</xml_diff>